<commit_message>
Add SearchAndReplaceExcelParams class and update package references
</commit_message>
<xml_diff>
--- a/ConsoleApp1/ConsoleApp1/data.xlsx
+++ b/ConsoleApp1/ConsoleApp1/data.xlsx
@@ -14,21 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
-    <t xml:space="preserve">NewText1</t>
+    <t xml:space="preserve">yes babe</t>
   </si>
   <si>
     <t xml:space="preserve">NewText2</t>
   </si>
   <si>
-    <t xml:space="preserve">OldText1</t>
-  </si>
-  <si>
     <t xml:space="preserve">ReplacedValue</t>
   </si>
   <si>
-    <t xml:space="preserve">yes baby</t>
+    <t xml:space="preserve">yes Baby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes Babe</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -532,7 +532,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>